<commit_message>
wrapping lampiran and code
</commit_message>
<xml_diff>
--- a/No8.xlsx
+++ b/No8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AW\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LMS\mik\ml\pr1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5D2D36-5FE5-4D0D-8C00-569BA668EE25}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A48171-E231-43F2-B271-D4F54C78EFA6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{1DAA6E72-52FA-4174-A8D3-76530EE4DDA3}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +159,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +197,18 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,22 +216,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -522,114 +583,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9886BB-3547-4423-8287-F9C9341ECC9C}">
   <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>5.0999999999999996</v>
       </c>
@@ -746,7 +805,7 @@
         <f>$AG$2*AC2*B2</f>
         <v>-1.0317904842388041E-3</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="5">
         <v>0.3</v>
       </c>
     </row>
@@ -1015,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D4:D14" si="28">D4+Y4</f>
+        <f t="shared" ref="D5:D14" si="28">D4+Y4</f>
         <v>9.7761133049695359E-2</v>
       </c>
       <c r="E5" s="1">
@@ -2218,5 +2277,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>